<commit_message>
Informe v3 falta chequear resumen y dar formatos
</commit_message>
<xml_diff>
--- a/segunda-parte/doc/Automatas.xlsx
+++ b/segunda-parte/doc/Automatas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54911\Documents\GitHub\Sondas\segunda-parte\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9172D2-D5C9-4962-ABAC-DA9BCC6FF951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C2BFB-FA92-4D18-A432-27382F52C13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4870DAD6-7886-456B-8B92-DF10D28B50A5}"/>
   </bookViews>
@@ -527,46 +527,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7632C59F-526A-462B-8ABE-D5066CB485BB}">
   <dimension ref="B1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,15 +985,15 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
@@ -1160,17 +1160,17 @@
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="22"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -1377,110 +1377,110 @@
     </row>
     <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="28"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="26"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="27"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="27"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="27"/>
+      <c r="F29" s="19"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="27"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="27"/>
+      <c r="F31" s="19"/>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="28"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="26"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="23"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
@@ -1490,7 +1490,7 @@
         <v>81</v>
       </c>
       <c r="D36" s="16"/>
-      <c r="E36" s="27"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
@@ -1500,7 +1500,7 @@
         <v>82</v>
       </c>
       <c r="D37" s="16"/>
-      <c r="E37" s="27"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
@@ -1510,7 +1510,7 @@
         <v>83</v>
       </c>
       <c r="D38" s="16"/>
-      <c r="E38" s="27"/>
+      <c r="E38" s="19"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
@@ -1520,7 +1520,7 @@
         <v>84</v>
       </c>
       <c r="D39" s="16"/>
-      <c r="E39" s="27"/>
+      <c r="E39" s="19"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
@@ -1530,40 +1530,40 @@
         <v>79</v>
       </c>
       <c r="D40" s="16"/>
-      <c r="E40" s="27"/>
+      <c r="E40" s="19"/>
     </row>
     <row r="41" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="19"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
     </row>
     <row r="42" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="22"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="26"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25" t="s">
+      <c r="D44" s="15"/>
+      <c r="E44" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="F44" s="26"/>
+      <c r="F44" s="23"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
@@ -1576,7 +1576,7 @@
       <c r="E45" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="27"/>
+      <c r="F45" s="19"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
@@ -1589,7 +1589,7 @@
       <c r="E46" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="F46" s="27"/>
+      <c r="F46" s="19"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
@@ -1602,7 +1602,7 @@
       <c r="E47" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F47" s="27"/>
+      <c r="F47" s="19"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
@@ -1615,7 +1615,7 @@
       <c r="E48" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F48" s="27"/>
+      <c r="F48" s="19"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
@@ -1628,27 +1628,27 @@
       <c r="E49" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F49" s="27"/>
+      <c r="F49" s="19"/>
     </row>
     <row r="50" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18" t="s">
+      <c r="D50" s="17"/>
+      <c r="E50" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F50" s="19"/>
+      <c r="F50" s="18"/>
     </row>
     <row r="51" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="24"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="3" t="s">
         <v>12</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="27" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="16"/>
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="27" t="s">
         <v>76</v>
       </c>
       <c r="C54" s="16"/>
@@ -1726,7 +1726,7 @@
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="27" t="s">
         <v>77</v>
       </c>
       <c r="C55" s="16"/>
@@ -1753,7 +1753,7 @@
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="27" t="s">
         <v>78</v>
       </c>
       <c r="C56" s="16"/>
@@ -1780,7 +1780,7 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="27" t="s">
         <v>79</v>
       </c>
       <c r="C57" s="16"/>
@@ -1807,10 +1807,10 @@
       </c>
     </row>
     <row r="58" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="18"/>
+      <c r="C58" s="17"/>
       <c r="D58" s="9" t="s">
         <v>10</v>
       </c>
@@ -1835,13 +1835,27 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="B7:H7"/>
@@ -1858,28 +1872,14 @@
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="E50:F50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>